<commit_message>
added values for records which were only ID'd at genus level
</commit_message>
<xml_diff>
--- a/data/missing and mismatched.xlsx
+++ b/data/missing and mismatched.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="477">
   <si>
     <t>Species</t>
   </si>
@@ -1407,9 +1407,6 @@
     <t>need data, very common</t>
   </si>
   <si>
-    <t>not sure how to approach, M. quinquenervia is similar to bracteata, with larger leaves</t>
-  </si>
-  <si>
     <t>see Callerya</t>
   </si>
   <si>
@@ -1419,9 +1416,6 @@
     <t>common, but not possible to assign data to</t>
   </si>
   <si>
-    <t>v. common at some sites, need to assign some data</t>
-  </si>
-  <si>
     <t xml:space="preserve">common at one site. Likely planted, ignore. </t>
   </si>
   <si>
@@ -1441,6 +1435,27 @@
   </si>
   <si>
     <t>spelling</t>
+  </si>
+  <si>
+    <t>just use lomandra longifolia…</t>
+  </si>
+  <si>
+    <t>not sure how to approach, M. quinquenervia is similar to bracteata, with larger leaves. Jus t average…</t>
+  </si>
+  <si>
+    <t>v. common at some sites, need to assign some data. Just avg a few ripogonums</t>
+  </si>
+  <si>
+    <t>avged data?</t>
+  </si>
+  <si>
+    <t>?????</t>
+  </si>
+  <si>
+    <t>use cyperus involucratus data, but label as native</t>
+  </si>
+  <si>
+    <t>use carex appressa data</t>
   </si>
 </sst>
 </file>
@@ -1820,8 +1835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D244"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="E95" sqref="E95"/>
+    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
+      <selection activeCell="C185" sqref="C185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1859,7 +1874,7 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2158,6 +2173,9 @@
       <c r="A43" s="5" t="s">
         <v>186</v>
       </c>
+      <c r="D43" t="s">
+        <v>476</v>
+      </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
@@ -2327,7 +2345,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>47</v>
       </c>
@@ -2335,7 +2353,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>48</v>
       </c>
@@ -2343,7 +2361,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>49</v>
       </c>
@@ -2351,7 +2369,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>50</v>
       </c>
@@ -2359,7 +2377,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>51</v>
       </c>
@@ -2367,7 +2385,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>52</v>
       </c>
@@ -2375,7 +2393,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>53</v>
       </c>
@@ -2383,7 +2401,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>54</v>
       </c>
@@ -2391,7 +2409,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>55</v>
       </c>
@@ -2399,7 +2417,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>56</v>
       </c>
@@ -2407,12 +2425,15 @@
         <v>307</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D75" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>189</v>
       </c>
@@ -2420,7 +2441,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>57</v>
       </c>
@@ -2428,7 +2449,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>58</v>
       </c>
@@ -2436,7 +2457,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>209</v>
       </c>
@@ -2444,7 +2465,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
         <v>210</v>
       </c>
@@ -2577,10 +2598,10 @@
         <v>327</v>
       </c>
       <c r="D96" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>72</v>
       </c>
@@ -2588,7 +2609,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>73</v>
       </c>
@@ -2596,7 +2617,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>74</v>
       </c>
@@ -2604,7 +2625,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>75</v>
       </c>
@@ -2612,7 +2633,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>76</v>
       </c>
@@ -2620,7 +2641,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>77</v>
       </c>
@@ -2628,7 +2649,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>78</v>
       </c>
@@ -2636,7 +2657,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>79</v>
       </c>
@@ -2644,7 +2665,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>80</v>
       </c>
@@ -2652,7 +2673,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>81</v>
       </c>
@@ -2660,12 +2681,15 @@
         <v>337</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D107" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>82</v>
       </c>
@@ -2673,7 +2697,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>83</v>
       </c>
@@ -2681,7 +2705,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>84</v>
       </c>
@@ -2689,7 +2713,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>85</v>
       </c>
@@ -2697,7 +2721,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>86</v>
       </c>
@@ -2705,7 +2729,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>87</v>
       </c>
@@ -2713,7 +2737,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>88</v>
       </c>
@@ -2721,7 +2745,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>214</v>
       </c>
@@ -2729,7 +2753,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>89</v>
       </c>
@@ -2737,7 +2761,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>215</v>
       </c>
@@ -2745,7 +2769,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>90</v>
       </c>
@@ -2753,12 +2777,15 @@
         <v>348</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D119" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>91</v>
       </c>
@@ -2766,7 +2793,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>92</v>
       </c>
@@ -2774,7 +2801,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>93</v>
       </c>
@@ -2782,7 +2809,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>94</v>
       </c>
@@ -2790,7 +2817,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>95</v>
       </c>
@@ -2798,7 +2825,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>96</v>
       </c>
@@ -2806,7 +2833,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>216</v>
       </c>
@@ -2814,7 +2841,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>97</v>
       </c>
@@ -2822,7 +2849,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>98</v>
       </c>
@@ -2830,7 +2857,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>217</v>
       </c>
@@ -2838,7 +2865,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>99</v>
       </c>
@@ -2846,7 +2873,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>100</v>
       </c>
@@ -2854,7 +2881,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>101</v>
       </c>
@@ -2862,12 +2889,15 @@
         <v>361</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="4" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D133" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>102</v>
       </c>
@@ -2875,7 +2905,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>218</v>
       </c>
@@ -2883,7 +2913,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>103</v>
       </c>
@@ -2891,7 +2921,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>104</v>
       </c>
@@ -2899,7 +2929,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>105</v>
       </c>
@@ -2907,7 +2937,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>106</v>
       </c>
@@ -2915,22 +2945,25 @@
         <v>367</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="6" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D141" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>195</v>
       </c>
@@ -2938,7 +2971,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>109</v>
       </c>
@@ -3047,7 +3080,7 @@
         <v>116</v>
       </c>
       <c r="D157" t="s">
-        <v>460</v>
+        <v>471</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
@@ -3087,7 +3120,7 @@
         <v>224</v>
       </c>
       <c r="D162" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
@@ -3140,7 +3173,7 @@
         <v>126</v>
       </c>
       <c r="D169" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
@@ -3417,7 +3450,7 @@
         <v>233</v>
       </c>
       <c r="D204" t="s">
-        <v>464</v>
+        <v>472</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
@@ -3425,7 +3458,7 @@
         <v>154</v>
       </c>
       <c r="D205" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
@@ -3449,7 +3482,7 @@
         <v>234</v>
       </c>
       <c r="D208" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
@@ -3473,7 +3506,7 @@
         <v>197</v>
       </c>
       <c r="D211" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
@@ -3481,7 +3514,7 @@
         <v>157</v>
       </c>
       <c r="D212" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
@@ -3585,7 +3618,7 @@
         <v>167</v>
       </c>
       <c r="D225" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
@@ -3633,7 +3666,7 @@
         <v>173</v>
       </c>
       <c r="D231" s="8" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fixed errors in trait dataset, working on exotics analysis
</commit_message>
<xml_diff>
--- a/data/missing and mismatched.xlsx
+++ b/data/missing and mismatched.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="477">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="478">
   <si>
     <t>Species</t>
   </si>
@@ -1456,6 +1456,9 @@
   </si>
   <si>
     <t>use carex appressa data</t>
+  </si>
+  <si>
+    <t>reeallly common</t>
   </si>
 </sst>
 </file>
@@ -1835,8 +1838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D244"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
-      <selection activeCell="C185" sqref="C185"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A80" sqref="A80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2959,8 +2962,11 @@
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
+      <c r="A142" s="5" t="s">
         <v>194</v>
+      </c>
+      <c r="D142" t="s">
+        <v>477</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>